<commit_message>
v. 1.0.1 with www beta
</commit_message>
<xml_diff>
--- a/Svai/7_4.xlsx
+++ b/Svai/7_4.xlsx
@@ -183,13 +183,13 @@
     <t>731</t>
   </si>
   <si>
-    <t xml:space="preserve">в глинистые грунты с показателем текучести 0,5</t>
+    <t xml:space="preserve">в глинистые грунты с показателем текучести меньше 0,5</t>
   </si>
   <si>
     <t>740</t>
   </si>
   <si>
-    <t xml:space="preserve">то же, 0,5</t>
+    <t xml:space="preserve">в глинистые грунты с показателем текучести болше 0,5</t>
   </si>
   <si>
     <t>end</t>
@@ -366,8 +366,8 @@
     <xf fontId="1" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1020,7 +1020,7 @@
       </c>
     </row>
     <row ht="38.25" r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -1040,7 +1040,7 @@
       </c>
     </row>
     <row ht="25.5" r="12">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -1060,7 +1060,7 @@
       </c>
     </row>
     <row ht="25.5" r="13">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -1080,7 +1080,7 @@
       </c>
     </row>
     <row ht="25.5" r="14">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="14" t="s">
@@ -1100,7 +1100,7 @@
       </c>
     </row>
     <row ht="25.5" r="15">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -1120,7 +1120,7 @@
       </c>
     </row>
     <row ht="25.5" r="16">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row ht="25.5" r="17">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -1158,7 +1158,7 @@
       </c>
     </row>
     <row ht="25.5" r="18">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1266,7 +1266,7 @@
       </c>
     </row>
     <row ht="14.25" r="24">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="14" t="s">
@@ -1283,8 +1283,8 @@
         <v>0.80000000000000004</v>
       </c>
     </row>
-    <row ht="25.5" r="25">
-      <c r="A25" s="10" t="s">
+    <row ht="38.25" r="25">
+      <c r="A25" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -1301,14 +1301,14 @@
         <v>1</v>
       </c>
     </row>
-    <row ht="14.25" r="26">
-      <c r="A26" s="10" t="s">
+    <row ht="38.25" r="26">
+      <c r="A26" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="14" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="12"/>

</xml_diff>